<commit_message>
export_metadata now adds rows for multiple entries on one row
</commit_message>
<xml_diff>
--- a/devel/Type source files/Gear_types.xlsx
+++ b/devel/Type source files/Gear_types.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Bottle</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Knife</t>
   </si>
   <si>
-    <t>Limnos</t>
-  </si>
-  <si>
     <t>Niskin bottle</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Suction pump</t>
   </si>
   <si>
-    <t>Swim-net</t>
-  </si>
-  <si>
     <t>Tucker trawl</t>
   </si>
   <si>
@@ -120,13 +114,22 @@
   </si>
   <si>
     <t>Ice corer 9 cm</t>
+  </si>
+  <si>
+    <t>duplicate name</t>
+  </si>
+  <si>
+    <t>Limnos water sampler</t>
+  </si>
+  <si>
+    <t>Swimnet 200 µm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +147,21 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,15 +187,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,171 +477,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.6640625" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:B30">
+    <sortCondition ref="A2:A30"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added CDOM data processing
</commit_message>
<xml_diff>
--- a/devel/Type source files/Gear_types.xlsx
+++ b/devel/Type source files/Gear_types.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikko\Dropbox\Workstuff\R\R packages\MarineDatabase\devel\Type source files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anette\Dropbox\Type source files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>Bottle</t>
   </si>
@@ -123,13 +123,108 @@
   </si>
   <si>
     <t>WP2 64 μm</t>
+  </si>
+  <si>
+    <t>Niskin</t>
+  </si>
+  <si>
+    <t>WP3 1000</t>
+  </si>
+  <si>
+    <t>MIK</t>
+  </si>
+  <si>
+    <t>WP2 500</t>
+  </si>
+  <si>
+    <t>plankton net</t>
+  </si>
+  <si>
+    <t>CTD</t>
+  </si>
+  <si>
+    <t>Multinet; MPS</t>
+  </si>
+  <si>
+    <t>Water bottle 10l</t>
+  </si>
+  <si>
+    <t>OLD GEAR</t>
+  </si>
+  <si>
+    <t>Mega zooplankton net 1.55</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">check wich sample type, could be Handnet 20 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µm</t>
+    </r>
+  </si>
+  <si>
+    <t>WP2 180; WP2 200</t>
+  </si>
+  <si>
+    <t>Diver</t>
+  </si>
+  <si>
+    <t>20 μm net; 20μm net; Phytoplankton net</t>
+  </si>
+  <si>
+    <t>juday net</t>
+  </si>
+  <si>
+    <t>Grab</t>
+  </si>
+  <si>
+    <t>bucket; sieve/Jar; Surface</t>
+  </si>
+  <si>
+    <t>hand net; Square net</t>
+  </si>
+  <si>
+    <t>WP2 150</t>
+  </si>
+  <si>
+    <t>Ice core</t>
+  </si>
+  <si>
+    <t>same as "Macro zooplankton net"; keep one of the names</t>
+  </si>
+  <si>
+    <t>WP2 63; WP2 63μm; WP2 60um</t>
+  </si>
+  <si>
+    <t>Bongo</t>
+  </si>
+  <si>
+    <t>RP sledge</t>
+  </si>
+  <si>
+    <t>suction pump; suction pump &amp; net</t>
+  </si>
+  <si>
+    <t>Divers; Divers; Snorkling</t>
+  </si>
+  <si>
+    <t>delete if no sample is attached</t>
+  </si>
+  <si>
+    <t>replace existin gear in database</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +260,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -477,173 +578,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.453125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.6328125" style="4"/>
+    <col min="1" max="1" width="24.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>24</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C36" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C37" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C38" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C39" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes to export_metadata
</commit_message>
<xml_diff>
--- a/devel/Type source files/Gear_types.xlsx
+++ b/devel/Type source files/Gear_types.xlsx
@@ -1,33 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anette\Dropbox\Type source files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15465"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="old gear" sheetId="2" r:id="rId2"/>
+    <sheet name="gear_type test" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="80">
   <si>
     <t>Bottle</t>
   </si>
@@ -187,9 +184,6 @@
     <t>bucket; sieve/Jar; Surface</t>
   </si>
   <si>
-    <t>hand net; Square net</t>
-  </si>
-  <si>
     <t>WP2 150</t>
   </si>
   <si>
@@ -217,14 +211,77 @@
     <t>delete if no sample is attached</t>
   </si>
   <si>
-    <t>replace existin gear in database</t>
+    <t>Arg</t>
+  </si>
+  <si>
+    <t>Bukcet</t>
+  </si>
+  <si>
+    <t>bottle</t>
+  </si>
+  <si>
+    <t>Go Flo</t>
+  </si>
+  <si>
+    <t>Handnet 20μm</t>
+  </si>
+  <si>
+    <t>Hydrobios CTD</t>
+  </si>
+  <si>
+    <t>Ice corer 14cm</t>
+  </si>
+  <si>
+    <t>Ice corer 9cm</t>
+  </si>
+  <si>
+    <t>knife</t>
+  </si>
+  <si>
+    <t>Water sampler</t>
+  </si>
+  <si>
+    <t>plastic net</t>
+  </si>
+  <si>
+    <t>MIK-net 1500µm</t>
+  </si>
+  <si>
+    <t>Multinet 200</t>
+  </si>
+  <si>
+    <t>Multinet 64ym</t>
+  </si>
+  <si>
+    <t>niskin</t>
+  </si>
+  <si>
+    <t>baited trap</t>
+  </si>
+  <si>
+    <t>WP2 150µm</t>
+  </si>
+  <si>
+    <t>WP2 200µm</t>
+  </si>
+  <si>
+    <t>WP2 500µm</t>
+  </si>
+  <si>
+    <t>WP2 64m</t>
+  </si>
+  <si>
+    <t>WP3 1000μm</t>
+  </si>
+  <si>
+    <t>snorkel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +324,29 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -285,10 +365,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -298,8 +388,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,7 +671,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -578,284 +679,223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.5703125" style="4"/>
+    <col min="1" max="1" width="24.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.5" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C33" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C34" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C35" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C36" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C37" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C38" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C39" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>58</v>
+      <c r="B31" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -863,7 +903,406 @@
     <sortCondition ref="A2:A30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>